<commit_message>
17/12/24 mant producto y demas
</commit_message>
<xml_diff>
--- a/docs/Data-InformacioDemo.xlsx
+++ b/docs/Data-InformacioDemo.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PERSONAL_CompraVenta\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC633E4-1BB7-4023-A7BF-A93EF406452D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D88EF3-1533-4168-A615-23CEF891A3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7179417F-1222-415C-A875-6DA2BAFD3F05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{7179417F-1222-415C-A875-6DA2BAFD3F05}"/>
   </bookViews>
   <sheets>
     <sheet name="Categoria" sheetId="1" r:id="rId1"/>
     <sheet name="Moneda" sheetId="2" r:id="rId2"/>
     <sheet name="Unidad" sheetId="3" r:id="rId3"/>
+    <sheet name="Cliente" sheetId="4" r:id="rId4"/>
+    <sheet name="Proveedor" sheetId="5" r:id="rId5"/>
+    <sheet name="Producto" sheetId="6" r:id="rId6"/>
+    <sheet name="Rol" sheetId="7" r:id="rId7"/>
+    <sheet name="Menu" sheetId="8" r:id="rId8"/>
+    <sheet name="Menu Detalle" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="131">
   <si>
     <t>CAT_ID</t>
   </si>
@@ -80,12 +86,12 @@
     <t>MON_NOM</t>
   </si>
   <si>
+    <t>SOL</t>
+  </si>
+  <si>
     <t>DOL</t>
   </si>
   <si>
-    <t>GUA</t>
-  </si>
-  <si>
     <t>UND_ID</t>
   </si>
   <si>
@@ -102,19 +108,364 @@
   </si>
   <si>
     <t>Kilos</t>
+  </si>
+  <si>
+    <t>CLI_ID</t>
+  </si>
+  <si>
+    <t>EMP_ID</t>
+  </si>
+  <si>
+    <t>CLI_NOM</t>
+  </si>
+  <si>
+    <t>CLI_RUC</t>
+  </si>
+  <si>
+    <t>CLI_TELF</t>
+  </si>
+  <si>
+    <t>CLI_DIRECC</t>
+  </si>
+  <si>
+    <t>CLI_CORREO</t>
+  </si>
+  <si>
+    <t>Pepito SA</t>
+  </si>
+  <si>
+    <t>av siempre viva nro 99</t>
+  </si>
+  <si>
+    <t>cliente1@clientetest.com</t>
+  </si>
+  <si>
+    <t>Jorgito SAC</t>
+  </si>
+  <si>
+    <t>av siempre viva nro 100</t>
+  </si>
+  <si>
+    <t>av siempre viva nro 101</t>
+  </si>
+  <si>
+    <t>cliente2@clientetest.com</t>
+  </si>
+  <si>
+    <t>Casillo EIRL</t>
+  </si>
+  <si>
+    <t>PROV_ID</t>
+  </si>
+  <si>
+    <t>PROV_NOM</t>
+  </si>
+  <si>
+    <t>PROV_RUC</t>
+  </si>
+  <si>
+    <t>PROV_TELF</t>
+  </si>
+  <si>
+    <t>PROV_DIRECC</t>
+  </si>
+  <si>
+    <t>PROV_CORREO</t>
+  </si>
+  <si>
+    <t>Platanitos SA</t>
+  </si>
+  <si>
+    <t>777 4341</t>
+  </si>
+  <si>
+    <t>av buenos aires nro 99</t>
+  </si>
+  <si>
+    <t>proveedor1@proveedor.com</t>
+  </si>
+  <si>
+    <t>av buenos aires nro 100</t>
+  </si>
+  <si>
+    <t>av buenos aires nro 101</t>
+  </si>
+  <si>
+    <t>KFC EIRL</t>
+  </si>
+  <si>
+    <t>Popeye SAC</t>
+  </si>
+  <si>
+    <t>778 4342</t>
+  </si>
+  <si>
+    <t>779 4343</t>
+  </si>
+  <si>
+    <t>av buenos aires nro 102</t>
+  </si>
+  <si>
+    <t>780 4344</t>
+  </si>
+  <si>
+    <t>Bembos SAC</t>
+  </si>
+  <si>
+    <t>proveedor2@proveedor.com</t>
+  </si>
+  <si>
+    <t>proveedor3@proveedor.com</t>
+  </si>
+  <si>
+    <t>proveedor4@proveedor.com</t>
+  </si>
+  <si>
+    <t>PROD_ID</t>
+  </si>
+  <si>
+    <t>PROD_NOM</t>
+  </si>
+  <si>
+    <t>PROD_DESCRIP</t>
+  </si>
+  <si>
+    <t>PROD_PCOMPRA</t>
+  </si>
+  <si>
+    <t>PROD_PVENTA</t>
+  </si>
+  <si>
+    <t>PROD_STOCK</t>
+  </si>
+  <si>
+    <t>PROD_FECHAVEN</t>
+  </si>
+  <si>
+    <t>PROD_IMG</t>
+  </si>
+  <si>
+    <t>Branded T-Shirts</t>
+  </si>
+  <si>
+    <t>Borosil Paper Cup</t>
+  </si>
+  <si>
+    <t>Stillbird Helmet</t>
+  </si>
+  <si>
+    <t>Branded T-Shirts S</t>
+  </si>
+  <si>
+    <t>Branded T-Shirts M</t>
+  </si>
+  <si>
+    <t>Branded T-Shirts L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bentwood Chair </t>
+  </si>
+  <si>
+    <t>Bentwood Chair S</t>
+  </si>
+  <si>
+    <t>Bentwood Chair M</t>
+  </si>
+  <si>
+    <t>Branded T-Shirts XL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One Seater Sofa </t>
+  </si>
+  <si>
+    <t>One Seater Sofa S</t>
+  </si>
+  <si>
+    <t>Branded T-Shirts XS</t>
+  </si>
+  <si>
+    <t>Bentwood Chair XS</t>
+  </si>
+  <si>
+    <t>Stillbird Helmet S</t>
+  </si>
+  <si>
+    <t>ROL_ID</t>
+  </si>
+  <si>
+    <t>ROL_NOM</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>Comprador</t>
+  </si>
+  <si>
+    <t>MEN_ID</t>
+  </si>
+  <si>
+    <t>MEN_NOM</t>
+  </si>
+  <si>
+    <t>MEN_RUTA</t>
+  </si>
+  <si>
+    <t>MEN_IDENTI</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>../home/</t>
+  </si>
+  <si>
+    <t>dashboard</t>
+  </si>
+  <si>
+    <t>Mnt.Categoria</t>
+  </si>
+  <si>
+    <t>../MntCategoria/</t>
+  </si>
+  <si>
+    <t>mntcategoria</t>
+  </si>
+  <si>
+    <t>../MntProducto/</t>
+  </si>
+  <si>
+    <t>Mnt.Producto</t>
+  </si>
+  <si>
+    <t>mntproducto</t>
+  </si>
+  <si>
+    <t>Mnt.Cliente</t>
+  </si>
+  <si>
+    <t>../MntCliente/</t>
+  </si>
+  <si>
+    <t>mntcliente</t>
+  </si>
+  <si>
+    <t>../MntProveedor/</t>
+  </si>
+  <si>
+    <t>Mnt.Proveedor</t>
+  </si>
+  <si>
+    <t>mntproveedor</t>
+  </si>
+  <si>
+    <t>../MntMoneda/</t>
+  </si>
+  <si>
+    <t>Mnt.Moneda</t>
+  </si>
+  <si>
+    <t>mntmoneda</t>
+  </si>
+  <si>
+    <t>Mnt.UndMedida</t>
+  </si>
+  <si>
+    <t>../MntUndMedida/</t>
+  </si>
+  <si>
+    <t>mntundmedida</t>
+  </si>
+  <si>
+    <t>../MntEmpresa/</t>
+  </si>
+  <si>
+    <t>Mnt.Empresa</t>
+  </si>
+  <si>
+    <t>mntempresa</t>
+  </si>
+  <si>
+    <t>Mnt.Sucursal</t>
+  </si>
+  <si>
+    <t>../MntSucursal/</t>
+  </si>
+  <si>
+    <t>mntsucursal</t>
+  </si>
+  <si>
+    <t>Mnt.Usuario</t>
+  </si>
+  <si>
+    <t>../MntUsuario/</t>
+  </si>
+  <si>
+    <t>mntusuario</t>
+  </si>
+  <si>
+    <t>../MntRol/</t>
+  </si>
+  <si>
+    <t>Mnt.Rol</t>
+  </si>
+  <si>
+    <t>mntrol</t>
+  </si>
+  <si>
+    <t>MEND_ID</t>
+  </si>
+  <si>
+    <t>MEND_PERMI</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem Ipsum is simply dummy text </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,13 +485,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1149,11 +1508,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B539EBBE-57A6-4C44-8C55-E2CCCC4E201B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAAD0C4-2290-4EE0-A233-7AAA2F3161FA}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1191,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1202,7 +1561,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1213,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1224,7 +1583,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1235,7 +1594,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1246,7 +1605,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1257,7 +1616,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1268,7 +1627,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1279,7 +1638,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1290,7 +1649,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1301,7 +1660,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1313,11 +1672,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08EF8CAA-1C93-44FA-A65A-C197E829495A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B84621-5B3C-4AC0-9423-CC0A32DF1A49}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,4 +1965,1825 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D0F60B-6F2E-47B7-B9C4-425CACD6DAD6}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>123456789</v>
+      </c>
+      <c r="E2">
+        <v>1112222</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>123456790</v>
+      </c>
+      <c r="E3">
+        <v>1112223</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>123456791</v>
+      </c>
+      <c r="E4">
+        <v>1112224</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>123456789</v>
+      </c>
+      <c r="E5">
+        <v>1112222</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>123456790</v>
+      </c>
+      <c r="E6">
+        <v>1112223</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>123456791</v>
+      </c>
+      <c r="E7">
+        <v>1112224</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>123456789</v>
+      </c>
+      <c r="E8">
+        <v>1112222</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>123456790</v>
+      </c>
+      <c r="E9">
+        <v>1112223</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>123456791</v>
+      </c>
+      <c r="E10">
+        <v>1112224</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{B09B3988-7D32-41C7-9544-82C57B5C248C}"/>
+    <hyperlink ref="G3:G4" r:id="rId2" display="cliente1@clientetest.com" xr:uid="{AC847E8B-5DE1-4FF6-99EF-B13DB56B0635}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{E6743645-3A7B-4667-9432-52C8DF540B70}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{38AD35E4-F684-4715-8398-B3276EED6142}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{1FB35857-8500-4BC2-8C14-48A3E49B49A5}"/>
+    <hyperlink ref="G6:G7" r:id="rId6" display="cliente1@clientetest.com" xr:uid="{BB4647D5-1A18-4365-8978-3617A53E4C70}"/>
+    <hyperlink ref="G6" r:id="rId7" xr:uid="{CAB738A8-45E5-46AF-B2FF-27E6B6FE5D51}"/>
+    <hyperlink ref="G7" r:id="rId8" xr:uid="{755C1F01-BC77-4617-AA8F-1A4201A26C3D}"/>
+    <hyperlink ref="G8" r:id="rId9" xr:uid="{9CF8E27E-3A5E-4712-8F6E-FE5EBE5C1B82}"/>
+    <hyperlink ref="G9:G10" r:id="rId10" display="cliente1@clientetest.com" xr:uid="{1A8A7142-E95F-4712-9633-9A5E79E696C5}"/>
+    <hyperlink ref="G9" r:id="rId11" xr:uid="{314771E4-7DF8-49B5-9542-6A85E5B9DB6D}"/>
+    <hyperlink ref="G10" r:id="rId12" xr:uid="{62EBF10A-1B1B-409D-A153-A8846C005BD3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E1BAE8-21A6-4146-9EF3-AD3435EB2567}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2">
+        <v>1034112099</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <v>1034112100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>1034112101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>1034112102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6">
+        <v>1034112099</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
+        <v>1034112100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8">
+        <v>1034112101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9">
+        <v>1034112102</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>1034112099</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>1034112100</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12">
+        <v>1034112101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13">
+        <v>1034112102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{BEBA03E4-5C4C-4F0B-AA54-C681D0296042}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{5B3E5ADC-F084-4238-805C-633A9CC5A332}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{846AEB01-F17D-4937-8276-68D3745470A5}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{1345729A-B948-42C6-ACCC-0BA94E9D838F}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{F95D34B3-D126-4F8C-A3E0-EE673638EFC6}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{663944A8-2CC1-4CBF-B054-0FD0D855F7B8}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{107B97E1-96F4-47E5-B2E3-95A4AC3BC72B}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{AEC85C89-E7C6-4997-BE2B-E476914F17BD}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{C654B122-22AA-47BB-B40A-D976AF13B000}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{0F12F4D6-8D4A-45DA-B539-061C111D4E56}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{41A24372-72D1-4A3B-886A-2AF868D3ABFD}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{583CE3CA-7FF0-4480-A5FC-E6BC8A1180F5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6C011C-CCF5-464B-89CA-5B63E3BA37DA}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>1000</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3">
+        <v>1000</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>200</v>
+      </c>
+      <c r="J4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>1000</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>200</v>
+      </c>
+      <c r="J6">
+        <v>1000</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>1000</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <v>1000</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>200</v>
+      </c>
+      <c r="J9">
+        <v>1000</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>200</v>
+      </c>
+      <c r="J10">
+        <v>1000</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>200</v>
+      </c>
+      <c r="J11">
+        <v>1000</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>200</v>
+      </c>
+      <c r="J12">
+        <v>1000</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <v>200</v>
+      </c>
+      <c r="J13">
+        <v>1000</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>200</v>
+      </c>
+      <c r="J14">
+        <v>1000</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>200</v>
+      </c>
+      <c r="J15">
+        <v>1000</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>200</v>
+      </c>
+      <c r="J16">
+        <v>1000</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9E598D-6352-49CC-BC96-AE233EF50C04}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBB6BA8-7186-495B-9909-4510EDC45A58}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57033A82-8D45-473A-ACCF-FB466130ABE7}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>